<commit_message>
Estilos , excel y estili de la marca agregado
</commit_message>
<xml_diff>
--- a/src/assets/documents/preguntaObjetivasArriesgada.xlsx
+++ b/src/assets/documents/preguntaObjetivasArriesgada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sullc\Documents\TPI\Workspace\TPIntegrador\Angular\TPI-Front\src\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29133CCE-0D32-448D-994C-EC2044518D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F719286A-C5BD-4F4C-971D-50487287C959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="2" xr2:uid="{EA040AEE-35B0-4F5B-AEF3-29BB44B005B2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>nombre</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>""</t>
-  </si>
-  <si>
-    <t>  }</t>
   </si>
   <si>
     <t>Nivel De Conocimiento</t>
@@ -186,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,12 +231,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -265,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,9 +268,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -599,7 +589,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,10 +616,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -640,10 +630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B5289D-8738-4DA2-AC29-B8179EB99313}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +641,7 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -662,22 +652,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -688,10 +669,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E557A189-07BD-4DD4-AE4E-E2A608F405F0}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A8" sqref="A8:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,19 +708,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -747,19 +728,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -767,19 +748,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -787,39 +768,39 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>39</v>
+      <c r="B6" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -827,27 +808,21 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -858,10 +833,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8759312-058C-4473-8FFB-A755D6FBD3C0}">
-  <dimension ref="A1:L125"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +875,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -909,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2"/>
       <c r="L2" s="4"/>
@@ -922,7 +897,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -931,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2"/>
       <c r="L3" s="4"/>
@@ -944,7 +919,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -953,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2"/>
       <c r="L4" s="4"/>
@@ -966,7 +941,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -975,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="2"/>
       <c r="L5" s="4"/>
@@ -988,7 +963,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -997,7 +972,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2"/>
       <c r="L6" s="4"/>
@@ -1010,7 +985,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1019,7 +994,7 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="2"/>
       <c r="L7" s="2"/>
@@ -1032,7 +1007,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1041,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="2"/>
       <c r="L8" s="2"/>
@@ -1054,7 +1029,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1063,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="2"/>
       <c r="L9" s="2"/>
@@ -1076,7 +1051,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1085,7 +1060,7 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2"/>
       <c r="L10" s="2"/>
@@ -1098,7 +1073,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1107,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" s="2"/>
       <c r="L11" s="2"/>
@@ -1120,7 +1095,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1129,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" s="2"/>
       <c r="L12" s="2"/>
@@ -1142,7 +1117,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1151,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" s="2"/>
       <c r="L13" s="2"/>
@@ -1164,7 +1139,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1173,7 +1148,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I14" s="2"/>
       <c r="L14" s="2"/>
@@ -1186,7 +1161,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1195,7 +1170,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L15" s="2"/>
     </row>
@@ -1207,7 +1182,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1216,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I16" s="2"/>
       <c r="L16" s="2"/>
@@ -1229,7 +1204,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1238,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I17" s="2"/>
       <c r="L17" s="2"/>
@@ -1250,8 +1225,8 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>45</v>
+      <c r="C18" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -1260,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I18" s="2"/>
       <c r="L18" s="2"/>
@@ -1273,7 +1248,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1282,19 +1257,16 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I19" s="2"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
-      <c r="L20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="3"/>
       <c r="I21" s="2"/>
-      <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I22" s="2"/>
@@ -1303,263 +1275,126 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G25" s="4"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G26" s="4"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G27" s="4"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
+      <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G28" s="4"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G29" s="4"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G30" s="4"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="4"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="4"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G33" s="4"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="2"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C37" s="2"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="2"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="2"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C40" s="2"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="2"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="2"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="2"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="2"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="2"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C46" s="2"/>
-      <c r="G46" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="2"/>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C51" s="2"/>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C52" s="2"/>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="2"/>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="2"/>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="2"/>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="2"/>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="2"/>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="2"/>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="2"/>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.25">
@@ -1588,162 +1423,6 @@
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I73" s="2"/>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I74" s="2"/>
-    </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I75" s="2"/>
-    </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I76" s="2"/>
-    </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I77" s="2"/>
-    </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I78" s="2"/>
-    </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I79" s="2"/>
-    </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I81" s="2"/>
-    </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I82" s="2"/>
-    </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I83" s="2"/>
-    </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I84" s="2"/>
-    </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I85" s="2"/>
-    </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I86" s="2"/>
-    </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I87" s="2"/>
-    </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I88" s="2"/>
-    </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I89" s="2"/>
-    </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I90" s="2"/>
-    </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I91" s="2"/>
-    </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I92" s="2"/>
-    </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I93" s="2"/>
-    </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I94" s="2"/>
-    </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I95" s="2"/>
-    </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I96" s="2"/>
-    </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I97" s="2"/>
-    </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I98" s="2"/>
-    </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I99" s="2"/>
-    </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I100" s="2"/>
-    </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I101" s="2"/>
-    </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I102" s="2"/>
-    </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I103" s="2"/>
-    </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I104" s="2"/>
-    </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I105" s="2"/>
-    </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I106" s="2"/>
-    </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I107" s="2"/>
-    </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I108" s="2"/>
-    </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I109" s="2"/>
-    </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I110" s="2"/>
-    </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I111" s="2"/>
-    </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I112" s="2"/>
-    </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I113" s="2"/>
-    </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I114" s="2"/>
-    </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I115" s="2"/>
-    </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I116" s="2"/>
-    </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I117" s="2"/>
-    </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I118" s="2"/>
-    </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I119" s="2"/>
-    </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I120" s="2"/>
-    </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I121" s="2"/>
-    </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I122" s="2"/>
-    </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I123" s="2"/>
-    </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I124" s="2"/>
-    </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I125" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1752,23 +1431,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100641454CD1F1E6E428D478A5DC37BACE7" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ef1708d85dca7377bd826ec35b62ca84">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xmlns:ns4="7798dcc9-908f-468f-826a-c598f412d6fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="69e720de7d55d3231f99e1910e4c19d8" ns3:_="" ns4:_="">
     <xsd:import namespace="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
@@ -1957,32 +1619,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46D3E674-3079-48B5-BFCB-0E49FE180026}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7798dcc9-908f-468f-826a-c598f412d6fc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FE838D2-67DD-483F-BECE-425D67F53E63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7274836D-657B-48C7-97FD-AD88493854E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1999,4 +1653,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FE838D2-67DD-483F-BECE-425D67F53E63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46D3E674-3079-48B5-BFCB-0E49FE180026}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7798dcc9-908f-468f-826a-c598f412d6fc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Agregando modifcacion de estilos....
</commit_message>
<xml_diff>
--- a/src/assets/documents/preguntaObjetivasArriesgada.xlsx
+++ b/src/assets/documents/preguntaObjetivasArriesgada.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tpi2\git\TPI-Front\src\assets\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sullc\Documents\TPI\Workspace\TPIntegrador\Angular\TPI-Front\src\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCDC0E1-D9AE-4C83-BC1D-66134E699B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A566383E-3978-48C6-81A2-94AFA78D40FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1440" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{EA040AEE-35B0-4F5B-AEF3-29BB44B005B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{EA040AEE-35B0-4F5B-AEF3-29BB44B005B2}"/>
   </bookViews>
   <sheets>
     <sheet name="categoria" sheetId="1" r:id="rId1"/>
@@ -107,76 +107,76 @@
     <t>Test Conocimiento Arriesgado</t>
   </si>
   <si>
+    <t>A- El apalancamiento financiero se refiere a la inversión en activos libres de riesgo.</t>
+  </si>
+  <si>
+    <t>B- El apalancamiento financiero es el uso de deuda para aumentar la exposición a un activo y puede aumentar tanto la rentabilidad como el riesgo.</t>
+  </si>
+  <si>
+    <t>C- El apalancamiento financiero implica diversificar una cartera para reducir el riesgo.</t>
+  </si>
+  <si>
+    <t>A- Las opciones son activos de bajo riesgo que se utilizan para proteger una cartera contra pérdidas.</t>
+  </si>
+  <si>
+    <t>C- Las opciones son inversiones seguras que garantizan un rendimiento fijo.</t>
+  </si>
+  <si>
+    <t>C- La volatilidad se refiere a la seguridad de las inversiones en efectivo.</t>
+  </si>
+  <si>
+    <t>A- El análisis técnico se enfoca en el estudio de los estados financieros de las empresas y no es relevante para un inversor arriesgado.</t>
+  </si>
+  <si>
+    <t>C- El análisis técnico se centra en la evaluación de la gestión de riesgos y no en la predicción de precios.</t>
+  </si>
+  <si>
+    <t>C- Se utiliza para vender una inversión cuando se alcanza un precio objetivo.</t>
+  </si>
+  <si>
+    <t>B- El análisis técnico implica el estudio de los patrones de precios pasados y el volumen de operaciones para predecir movimientos futuros del mercado.</t>
+  </si>
+  <si>
+    <t>A- La volatilidad se refiere a la estabilidad de los precios de mercado.</t>
+  </si>
+  <si>
+    <t>B- La volatilidad se refiere a la variación de los precios de mercado con el tiempo.</t>
+  </si>
+  <si>
+    <t>A- Los eventos económicos y políticos  globales no tienen impacto en la volatilidad del mercado.</t>
+  </si>
+  <si>
+    <t>B- Los eventos económicos y políticos globales pueden aumentar la volatilidad del mercado.</t>
+  </si>
+  <si>
+    <t>C- Los eventos económicos y políticos globales no afectan a los mercados.</t>
+  </si>
+  <si>
+    <t>B- Se utiliza para beneficiarse de aumentos de precio potenciales con un desembolso inicial limitado.</t>
+  </si>
+  <si>
+    <t>A- Se utiliza para limitar las pérdidas en una inversión.</t>
+  </si>
+  <si>
+    <t>B- Las opciones se utilizan para especular o cubrir posiciones.</t>
+  </si>
+  <si>
     <t>¿Puede explicar el concepto de apalancamiento financiero y cómo puede afectar a la rentabilidad y el riesgo de una inversión?</t>
   </si>
   <si>
-    <t>A- El apalancamiento financiero se refiere a la inversión en activos libres de riesgo.</t>
-  </si>
-  <si>
-    <t>B- El apalancamiento financiero es el uso de deuda para aumentar la exposición a un activo y puede aumentar tanto la rentabilidad como el riesgo.</t>
-  </si>
-  <si>
-    <t>C- El apalancamiento financiero implica diversificar una cartera para reducir el riesgo.</t>
+    <t>¿Cómo afectan los eventos económicos y políticos globales a la volatilidad del mercado, y cómo puede un inversor arriesgado aprovechar estas situaciones?</t>
+  </si>
+  <si>
+    <t>¿Qué significa el término \"volatilidad\" en el contexto de las inversiones y por qué es importante para un inversor arriesgado?</t>
   </si>
   <si>
     <t>¿Qué son las opciones y cómo se pueden utilizar en una estrategia de inversión arriesgada?</t>
   </si>
   <si>
-    <t>A- Las opciones son activos de bajo riesgo que se utilizan para proteger una cartera contra pérdidas.</t>
-  </si>
-  <si>
-    <t>C- Las opciones son inversiones seguras que garantizan un rendimiento fijo.</t>
-  </si>
-  <si>
-    <t>¿Cómo afectan los eventos económicos y políticos globales a la volatilidad del mercado, y cómo puede un inversor arriesgado aprovechar estas situaciones?</t>
-  </si>
-  <si>
-    <t>¿Qué significa el término \"volatilidad\" en el contexto de las inversiones y por qué es importante para un inversor arriesgado?</t>
-  </si>
-  <si>
-    <t>C- La volatilidad se refiere a la seguridad de las inversiones en efectivo.</t>
-  </si>
-  <si>
     <t>¿Cuál es el propósito principal de utilizar una opción de compra (call option) en una estrategia de inversión arriesgada?</t>
   </si>
   <si>
     <t>¿Qué es el análisis técnico en el contexto de la inversión y cómo puede ser útil para un inversor arriesgado?</t>
-  </si>
-  <si>
-    <t>A- El análisis técnico se enfoca en el estudio de los estados financieros de las empresas y no es relevante para un inversor arriesgado.</t>
-  </si>
-  <si>
-    <t>C- El análisis técnico se centra en la evaluación de la gestión de riesgos y no en la predicción de precios.</t>
-  </si>
-  <si>
-    <t>C- Se utiliza para vender una inversión cuando se alcanza un precio objetivo.</t>
-  </si>
-  <si>
-    <t>B- El análisis técnico implica el estudio de los patrones de precios pasados y el volumen de operaciones para predecir movimientos futuros del mercado.</t>
-  </si>
-  <si>
-    <t>A- La volatilidad se refiere a la estabilidad de los precios de mercado.</t>
-  </si>
-  <si>
-    <t>B- La volatilidad se refiere a la variación de los precios de mercado con el tiempo.</t>
-  </si>
-  <si>
-    <t>A- Los eventos económicos y políticos  globales no tienen impacto en la volatilidad del mercado.</t>
-  </si>
-  <si>
-    <t>B- Los eventos económicos y políticos globales pueden aumentar la volatilidad del mercado.</t>
-  </si>
-  <si>
-    <t>C- Los eventos económicos y políticos globales no afectan a los mercados.</t>
-  </si>
-  <si>
-    <t>B- Se utiliza para beneficiarse de aumentos de precio potenciales con un desembolso inicial limitado.</t>
-  </si>
-  <si>
-    <t>A- Se utiliza para limitar las pérdidas en una inversión.</t>
-  </si>
-  <si>
-    <t>B- Las opciones se utilizan para especular o cubrir posiciones.</t>
   </si>
 </sst>
 </file>
@@ -580,18 +580,18 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,15 +624,15 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -663,18 +663,18 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="175.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="194.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -694,12 +694,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -714,12 +714,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -734,12 +734,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -754,12 +754,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -774,12 +774,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -794,12 +794,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -824,22 +824,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8759312-058C-4473-8FFB-A755D6FBD3C0}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="245.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="137.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.5546875" customWidth="1"/>
+    <col min="3" max="3" width="245.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="154.5703125" customWidth="1"/>
+    <col min="12" max="12" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -859,7 +859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -867,7 +867,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -876,12 +876,12 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -889,7 +889,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -898,12 +898,12 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="I3" s="2"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -911,7 +911,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -920,12 +920,12 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="I4" s="2"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -933,7 +933,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -942,12 +942,12 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -955,7 +955,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -964,12 +964,12 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I6" s="2"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -977,7 +977,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -986,12 +986,12 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -999,7 +999,7 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1008,12 +1008,12 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="I8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1030,12 +1030,12 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="I9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1052,12 +1052,12 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="I10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1074,12 +1074,12 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1096,12 +1096,12 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1118,12 +1118,12 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1140,12 +1140,12 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1162,11 +1162,11 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1183,12 +1183,12 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1205,12 +1205,12 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="I17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -1227,12 +1227,12 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="I18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1249,172 +1249,121 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="I19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I58" s="2"/>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I61" s="2"/>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I62" s="2"/>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I63" s="2"/>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I64" s="2"/>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I65" s="2"/>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I66" s="2"/>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I67" s="2"/>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I68" s="2"/>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I69" s="2"/>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I70" s="2"/>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I71" s="2"/>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I72" s="2"/>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I73" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1423,15 +1372,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100641454CD1F1E6E428D478A5DC37BACE7" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ef1708d85dca7377bd826ec35b62ca84">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xmlns:ns4="7798dcc9-908f-468f-826a-c598f412d6fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="69e720de7d55d3231f99e1910e4c19d8" ns3:_="" ns4:_="">
     <xsd:import namespace="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
@@ -1620,7 +1560,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xsi:nil="true"/>
@@ -1628,15 +1568,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FE838D2-67DD-483F-BECE-425D67F53E63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7274836D-657B-48C7-97FD-AD88493854E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1655,7 +1596,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46D3E674-3079-48B5-BFCB-0E49FE180026}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1670,4 +1611,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FE838D2-67DD-483F-BECE-425D67F53E63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>